<commit_message>
Added a new tab on the DMD datasets excel file. It includes PRIDE studies, and if processed data is available, provides direct links. Processed data has different formats depending on technology. Some formats might be better to use than others.
</commit_message>
<xml_diff>
--- a/inst/DMD datasets.xlsx
+++ b/inst/DMD datasets.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\08_pkgs\r4proteomics\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://firalis-my.sharepoint.com/personal/miguel_casanova_firalis_com/Documents/Bureau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36145F53-61A7-4F7E-BE92-6CB22D4CA672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="380" documentId="13_ncr:1_{36145F53-61A7-4F7E-BE92-6CB22D4CA672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFC4107F-9254-44A5-BA4B-1F02EDCB96F9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Public Datasets" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
   <si>
     <t>Dataset ID</t>
   </si>
@@ -154,6 +156,286 @@
   </si>
   <si>
     <t>ProteomeXchange via PRIDE (linked in paper)</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD054747</t>
+  </si>
+  <si>
+    <t>PXD054747</t>
+  </si>
+  <si>
+    <t>Proteomics analysis of the SIRT1 activating compound SRT2104 effect on tibialis anterior muscle in Duchenne muscular dystrophy</t>
+  </si>
+  <si>
+    <t>TIC</t>
+  </si>
+  <si>
+    <t>Mus musculus (mouse)</t>
+  </si>
+  <si>
+    <t>Access to processed data</t>
+  </si>
+  <si>
+    <t>PXD052728</t>
+  </si>
+  <si>
+    <t>in vivo-like scaffold-free 3D in vitro Models of Muscular Dystrophies: The Case for Anchored Cell Sheet Engineering in Personalized Medicine</t>
+  </si>
+  <si>
+    <t>Homo sapiens (human)</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD052728</t>
+  </si>
+  <si>
+    <t>No. Only raw material.</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2024/12/PXD052728/Search.rar</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>Yes. Use proteinGroups.txt file inside Search.rar</t>
+  </si>
+  <si>
+    <t>PXD052143</t>
+  </si>
+  <si>
+    <t>Cardio-metabolic and cytoskeletal proteomic signatures differentiate stress hypersensitivity in dystrophin-deficient mdx mice</t>
+  </si>
+  <si>
+    <t>Spectral Abundance Factor - SAF</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD052143</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD050694</t>
+  </si>
+  <si>
+    <t>PXD050694</t>
+  </si>
+  <si>
+    <t>Proteomic characterization of the molecular signature of congenital myopathies</t>
+  </si>
+  <si>
+    <t>PXD042227</t>
+  </si>
+  <si>
+    <t>One-line-fits-all: a knockdown strategy for rapid, generic and versatile modelling of muscular dystrophies in 3D-tissue-engineered-skeletal-muscle</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD042227</t>
+  </si>
+  <si>
+    <t>Yes. Use main_output_stijn.tsv file inside 	SEARCH_Fig3.zip</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2024/02/PXD042227/SEARCH_Fig3.zip</t>
+  </si>
+  <si>
+    <t>PXD039533</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD039533</t>
+  </si>
+  <si>
+    <t>Systemic deletion of DMD exon 51 rescues clinically severe Duchenne muscular dystrophy in a pig model lacking DMD exon 52</t>
+  </si>
+  <si>
+    <t>Sus scrofa domesticus (domestic pig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. </t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2023/07/PXD039533/proteinGroups_myocardium.txt</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2023/07/PXD039533/proteinGroups_triceps.txt</t>
+  </si>
+  <si>
+    <t>PXD038406</t>
+  </si>
+  <si>
+    <t>Atrogin-1 regulates BiP levels - novel therapeutic targets for Duchenne Muscular Dystrophy</t>
+  </si>
+  <si>
+    <t>Danio rerio (zebrafish) (brachydanio rerio)</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD038406</t>
+  </si>
+  <si>
+    <t>Yes. proteinGroups.txt inside Library.zip</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2024/03/PXD038406/Library.zip</t>
+  </si>
+  <si>
+    <t>PXD028886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paeonia lactiflora extract increase the muscle function via downregulation of high mobility group box 1 and NF-kB signaling in mdx mice, an animal model of Duchenne muscular dystrophy
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD028886</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2022/02/PXD028886/210128-ebiogen_Mouse_samples_SWATH_37m_wo_reanno_nofix.tsv</t>
+  </si>
+  <si>
+    <t>PXD027772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A scalable, clinically severe pig model for Duchenne muscular dystrophy
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD027772</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2021/12/PXD027772/Myocardium_proteinGroups.txt</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2021/12/PXD027772/SKM_proteinGroups.txt</t>
+  </si>
+  <si>
+    <t>PXD024631</t>
+  </si>
+  <si>
+    <t>STARS overexpression in the mdx mouse tibialis anterior muscle increases maximal isometric force production and regulates members of the keratin, NRF2 and OXPHOS pathways</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD024631</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2021/08/PXD024631/P30569_2D-IDA-All.group</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2021/08/PXD024631/P30569_2D-IDA-All_HumanDB.group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. 	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteome analysis of skeletal muscle samples from a porcine model of Duchenne muscular dystrophy
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD016003</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2020/01/PXD016003/proteinGroups.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myogenesis modelled by human pluripotent stem cells uncovers Duchenne muscular dystrophy phenotypes prior to skeletal muscle commitment
+</t>
+  </si>
+  <si>
+    <t>PXD015355</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD015355</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2021/09/PXD015355/24May18_Maxime_DMD_pep_all.xlsx</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2020/02/PXD014893/proteinGroups.txt</t>
+  </si>
+  <si>
+    <t>PXD014893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteome analysis of skeletal muscle samples from a porcine model of Duchenne muscular dystrophy treated by somatic gene editing
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD014893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis of skeletal muscle from a tailored pig model of Duchenne muscular dystrophy
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD002918</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2016/09/PXD002918/proteinGroups.txt</t>
+  </si>
+  <si>
+    <t>PXD059983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteome analysis of satellite cells from DMD and WT pigs
+</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/pride/archive/projects/PXD059983</t>
+  </si>
+  <si>
+    <t>https://ftp.pride.ebi.ac.uk/pride/data/archive/2025/06/PXD059983/proteinGroups.txt</t>
+  </si>
+  <si>
+    <t>Processing Software</t>
+  </si>
+  <si>
+    <t>Not usable</t>
+  </si>
+  <si>
+    <t>MaxQuant</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>DIA-NN</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>OpenSWATH/Unknown</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Spectronaut</t>
+  </si>
+  <si>
+    <t>TMT</t>
+  </si>
+  <si>
+    <t>Proteome Discoverer</t>
+  </si>
+  <si>
+    <t>Label free - LFQ</t>
+  </si>
+  <si>
+    <t>Data-independent acquisition - DIA/SWATH</t>
+  </si>
+  <si>
+    <t>MS1 intensity based label-free quantification method - LFQ</t>
+  </si>
+  <si>
+    <t>SWATH MS</t>
+  </si>
+  <si>
+    <t>Usability for the course</t>
+  </si>
+  <si>
+    <t>URI(s)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -220,6 +502,26 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -229,6 +531,11 @@
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{40A15EB6-10E8-4D1F-B122-7CD2BE8AAC9B}"/>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFF85D3E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -505,22 +812,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -566,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -589,7 +896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -612,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -635,7 +942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -658,7 +965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -692,4 +999,612 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2C6E54-5F11-41F7-B663-CDE5408E29DA}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="50.109375" customWidth="1"/>
+    <col min="11" max="11" width="53.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="6">
+        <v>45784</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="6">
+        <v>45650</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="6">
+        <v>45654</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="6">
+        <v>45783</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="6">
+        <v>45348</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6">
+        <v>45118</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="6">
+        <v>45358</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44608</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="6">
+        <v>44531</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6">
+        <v>44420</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="6">
+        <v>43839</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="6">
+        <v>44447</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="6">
+        <v>43866</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="6">
+        <v>42640</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="6">
+        <v>45837</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="3:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{2927A7A9-1EE0-4EC6-885B-0DD8C2B78CB0}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{932164C5-1C41-474F-AF5C-B9A1D7E43A19}"/>
+    <hyperlink ref="J3" r:id="rId3" xr:uid="{032619F2-43F3-4222-BCC9-F47B07D75D67}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{2630AAAA-A928-4E1A-8D81-AC807EE2A3C6}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{1A3C9F7C-CAF6-4A79-B1B9-2E6116999359}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{4309585F-87DC-45E8-A4A7-9039BD0C547A}"/>
+    <hyperlink ref="J6" r:id="rId7" xr:uid="{7C5ADC6F-C048-4F92-BD8E-E1CB031C231D}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{C63D783A-F3FF-40A4-A58D-3DE0FD0C5A19}"/>
+    <hyperlink ref="J7" r:id="rId9" xr:uid="{9A5DDF53-1576-4ED1-A06D-274D0911378D}"/>
+    <hyperlink ref="K7" r:id="rId10" xr:uid="{7D3F7AA9-BEF7-4F1A-B81A-3EE38505B8ED}"/>
+    <hyperlink ref="G8" r:id="rId11" xr:uid="{F97E77FC-19F9-44DA-B96A-5C5530CB794F}"/>
+    <hyperlink ref="J8" r:id="rId12" xr:uid="{4834EC96-30C1-49FB-9D0B-447AE578B745}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{6B0E7FD1-A4B5-4FFA-98AA-6B99ECB2E3E6}"/>
+    <hyperlink ref="J9" r:id="rId14" xr:uid="{C7FF56D0-FB7A-4637-B693-100232B40785}"/>
+    <hyperlink ref="G10" r:id="rId15" xr:uid="{7905ED4F-813D-4E5F-BDC3-18D0EE7A5881}"/>
+    <hyperlink ref="J10" r:id="rId16" xr:uid="{1C0AE016-7629-4CFD-9A3F-DB032F9C2ED0}"/>
+    <hyperlink ref="K10" r:id="rId17" xr:uid="{6F342FFF-4E13-406F-8828-C07114479532}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{843A33CA-220E-4F77-AD70-99B95008E859}"/>
+    <hyperlink ref="J11" r:id="rId19" xr:uid="{955178E9-3C6D-460B-B0B6-9FC148361549}"/>
+    <hyperlink ref="K11" r:id="rId20" xr:uid="{58096448-544C-448F-9920-52B131E5611E}"/>
+    <hyperlink ref="G12" r:id="rId21" xr:uid="{A01A4C70-1DC8-4133-81A6-36670514F912}"/>
+    <hyperlink ref="J12" r:id="rId22" xr:uid="{A71B5FF7-1985-47E7-9019-81EFAE8CF57E}"/>
+    <hyperlink ref="G13" r:id="rId23" xr:uid="{EC57E044-FE7D-4E7E-92BC-EFEDD36AA9BB}"/>
+    <hyperlink ref="J13" r:id="rId24" xr:uid="{FCA86411-4160-4EE8-80B5-60FA24915425}"/>
+    <hyperlink ref="J14" r:id="rId25" xr:uid="{0C1BD9CD-2899-405B-B20F-B57D8CF6E4D1}"/>
+    <hyperlink ref="G14" r:id="rId26" xr:uid="{993D56C5-E06D-4E3D-BCF7-974A313E8FC0}"/>
+    <hyperlink ref="G15" r:id="rId27" xr:uid="{95BECCA8-3AA7-496B-ADCD-7BC8127D87A4}"/>
+    <hyperlink ref="J15" r:id="rId28" xr:uid="{78ECBA9D-95EE-4E13-89D4-29BC39335A0D}"/>
+    <hyperlink ref="G16" r:id="rId29" xr:uid="{FC8B7163-43DE-4554-8FD4-B16A8FC12491}"/>
+    <hyperlink ref="J16" r:id="rId30" xr:uid="{51EC6520-17CC-418B-B5A4-A175DC755663}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>